<commit_message>
add report comment column to example docs
</commit_message>
<xml_diff>
--- a/inst/example_data/report_config.xlsx
+++ b/inst/example_data/report_config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomas.smith5\OneDrive - nuh.nhs.uk\Documents\R\R Package Development\ThomUK\SPCreporter\inst\example_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Tom Smith\Documents\R\R Projects\SPCreporter\inst\example_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC218CDA-03DE-4DBB-805A-A01673E4CB2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4635" windowHeight="4560"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="report_config" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>ref</t>
   </si>
@@ -69,12 +70,21 @@
   </si>
   <si>
     <t>Answers per day</t>
+  </si>
+  <si>
+    <t>report_comment</t>
+  </si>
+  <si>
+    <t>Recent points demonstrate special-cause improvement.  Congratulations and carry on!</t>
+  </si>
+  <si>
+    <t>This is a comment about the attendances metric.  This text is added via 'report_config.xlsx'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -385,22 +395,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="72.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,8 +424,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -427,8 +441,11 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5</v>
       </c>
@@ -442,7 +459,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10</v>
       </c>
@@ -456,7 +473,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>11</v>
       </c>
@@ -470,7 +487,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>16</v>
       </c>
@@ -484,7 +501,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>43</v>
       </c>
@@ -497,8 +514,11 @@
       <c r="D7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
reconfigure report_config to include spc_chart_type column
</commit_message>
<xml_diff>
--- a/inst/example_data/report_config.xlsx
+++ b/inst/example_data/report_config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francis.barton\Documents\R Projects\SPCreporter\inst\example_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Tom Smith\Documents\R\R Projects\SPCreporter\inst\example_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001D17A4-6C74-4BEC-8EE9-9080FF0716C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="4635" windowHeight="4560"/>
+    <workbookView xWindow="28680" yWindow="-6615" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="report_config" sheetId="1" r:id="rId1"/>
@@ -80,15 +81,6 @@
     <t>none</t>
   </si>
   <si>
-    <t>rare_event_chart</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>report_comment</t>
   </si>
   <si>
@@ -96,12 +88,21 @@
   </si>
   <si>
     <t>Recent points demonstrate special-cause improvement.  Congratulations and carry on!</t>
+  </si>
+  <si>
+    <t>spc_chart_type</t>
+  </si>
+  <si>
+    <t>xmr</t>
+  </si>
+  <si>
+    <t>t</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -412,22 +413,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="3.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="121" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,16 +439,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -458,16 +459,16 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5</v>
       </c>
@@ -478,13 +479,13 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10</v>
       </c>
@@ -495,13 +496,13 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>11</v>
       </c>
@@ -512,13 +513,13 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>16</v>
       </c>
@@ -529,13 +530,13 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>43</v>
       </c>
@@ -546,16 +547,16 @@
         <v>12</v>
       </c>
       <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
       <c r="F7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -566,13 +567,13 @@
         <v>12</v>
       </c>
       <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>99</v>
       </c>
@@ -583,13 +584,13 @@
         <v>16</v>
       </c>
       <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
         <v>6</v>
       </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>99</v>
       </c>
@@ -600,10 +601,10 @@
         <v>16</v>
       </c>
       <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
         <v>17</v>
-      </c>
-      <c r="E10" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>